<commit_message>
TB works, still need to finish SIR later
</commit_message>
<xml_diff>
--- a/atomica/core/framework_template.xlsx
+++ b/atomica/core/framework_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\atomica\core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA2A9A2-F290-4292-8C3E-4D6AB05B4885}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D39BD89-AC78-4932-85C9-EC70B4CCF490}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Databook Pages" sheetId="1" r:id="rId1"/>
@@ -722,7 +722,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="50">
   <si>
     <t>Datasheet Code Name</t>
   </si>
@@ -797,12 +797,6 @@
   </si>
   <si>
     <t>Is Impact</t>
-  </si>
-  <si>
-    <t>Abbreviation</t>
-  </si>
-  <si>
-    <t>Full name</t>
   </si>
   <si>
     <t>Type</t>
@@ -959,42 +953,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <fill>
         <patternFill>
@@ -1054,49 +1013,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1460,7 +1377,7 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -1480,23 +1397,23 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="22" priority="1">
+    <cfRule type="expression" dxfId="11" priority="1">
       <formula>AND(A1&lt;&gt;"",NOT(B1&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1512,7 +1429,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1563,7 +1480,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -1576,7 +1493,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -1586,12 +1503,12 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="21" priority="4">
+    <cfRule type="expression" dxfId="10" priority="4">
       <formula>AND(A1&lt;&gt;"",NOT(B1&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H1048576">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="9" priority="2">
       <formula>AND(I2&lt;&gt;"",NOT(H2&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1653,7 +1570,7 @@
   <sheetData>
     <row r="1" spans="1:398" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B1" s="3" t="str">
         <f>IF(Compartments!$A2&lt;&gt;"",Compartments!$A2,"")</f>
@@ -5659,7 +5576,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5730,12 +5647,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="expression" dxfId="11" priority="6">
+    <cfRule type="expression" dxfId="6" priority="6">
       <formula>AND(A2&lt;&gt;"",NOT(B2&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H1048576">
-    <cfRule type="expression" dxfId="10" priority="5">
+    <cfRule type="expression" dxfId="5" priority="5">
       <formula>AND(I2&lt;&gt;"",NOT(H2&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5787,7 +5704,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5840,10 +5757,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -5854,20 +5771,20 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="19" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>AND(A1&lt;&gt;"",NOT(B1&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J1048576">
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>AND(K2&lt;&gt;"",NOT(J2&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5944,10 +5861,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -5956,7 +5873,7 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="17" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>AND(A1&lt;&gt;"",NOT(B1&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5981,26 +5898,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -6012,8 +5929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6A2575B-90FD-4432-ABB5-1D1C9A3EC31C}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6028,61 +5945,66 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{B6FB0777-9CB4-4E7A-978E-F88EC2A52ADA}">
+      <formula1>"n,y"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add about sheet from which name is drawn
</commit_message>
<xml_diff>
--- a/atomica/core/framework_template.xlsx
+++ b/atomica/core/framework_template.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\atomica\core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D39BD89-AC78-4932-85C9-EC70B4CCF490}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F027DE4-6112-42CD-A7B4-6E6DD04DF68C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Databook Pages" sheetId="1" r:id="rId1"/>
-    <sheet name="Compartments" sheetId="2" r:id="rId2"/>
-    <sheet name="Transitions" sheetId="3" r:id="rId3"/>
-    <sheet name="Characteristics" sheetId="4" r:id="rId4"/>
-    <sheet name="Parameters" sheetId="6" r:id="rId5"/>
-    <sheet name="Interactions" sheetId="5" r:id="rId6"/>
-    <sheet name="Cascades" sheetId="7" r:id="rId7"/>
-    <sheet name="Plots" sheetId="8" r:id="rId8"/>
+    <sheet name="About" sheetId="9" r:id="rId1"/>
+    <sheet name="Databook Pages" sheetId="1" r:id="rId2"/>
+    <sheet name="Compartments" sheetId="2" r:id="rId3"/>
+    <sheet name="Transitions" sheetId="3" r:id="rId4"/>
+    <sheet name="Characteristics" sheetId="4" r:id="rId5"/>
+    <sheet name="Parameters" sheetId="6" r:id="rId6"/>
+    <sheet name="Interactions" sheetId="5" r:id="rId7"/>
+    <sheet name="Cascades" sheetId="7" r:id="rId8"/>
+    <sheet name="Plots" sheetId="8" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
@@ -722,7 +723,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="54">
   <si>
     <t>Datasheet Code Name</t>
   </si>
@@ -873,6 +874,18 @@
   <si>
     <t>Interaction 1</t>
   </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Template</t>
+  </si>
+  <si>
+    <t>This is a template cascade</t>
+  </si>
 </sst>
 </file>
 
@@ -934,7 +947,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -948,6 +961,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1371,14 +1387,53 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABBEF971-4BEF-4E47-AA22-99A396340633}">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+    <col min="2" max="2" width="74.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="234.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
-    <tabColor theme="9" tint="0.39997558519241921"/>
+    <tabColor theme="5" tint="0.79998168889431442"/>
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1421,10 +1476,10 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
-    <tabColor theme="9" tint="0.39997558519241921"/>
+    <tabColor theme="5" tint="0.79998168889431442"/>
   </sheetPr>
   <dimension ref="A1:K3"/>
   <sheetViews>
@@ -1552,10 +1607,10 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
-    <tabColor theme="9" tint="0.39997558519241921"/>
+    <tabColor theme="5" tint="0.79998168889431442"/>
   </sheetPr>
   <dimension ref="A1:OH398"/>
   <sheetViews>
@@ -5568,10 +5623,10 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
-    <tabColor theme="9" tint="0.39997558519241921"/>
+    <tabColor theme="5" tint="0.79998168889431442"/>
   </sheetPr>
   <dimension ref="A1:J3"/>
   <sheetViews>
@@ -5696,10 +5751,10 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
-    <tabColor theme="9" tint="0.39997558519241921"/>
+    <tabColor theme="5" tint="0.79998168889431442"/>
   </sheetPr>
   <dimension ref="A1:K3"/>
   <sheetViews>
@@ -5830,10 +5885,10 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
-    <tabColor theme="9" tint="0.39997558519241921"/>
+    <tabColor theme="5" tint="0.79998168889431442"/>
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -5882,7 +5937,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A1EAFB5-C4B0-491C-B03B-D10386E1B6D4}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -5925,11 +5980,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6A2575B-90FD-4432-ABB5-1D1C9A3EC31C}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add simple and advanced templates
</commit_message>
<xml_diff>
--- a/atomica/core/framework_template.xlsx
+++ b/atomica/core/framework_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\atomica\core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F027DE4-6112-42CD-A7B4-6E6DD04DF68C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B003D609-37F1-48F5-AB7E-2A3C78C86A81}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,15 +19,71 @@
     <sheet name="Transitions" sheetId="3" r:id="rId4"/>
     <sheet name="Characteristics" sheetId="4" r:id="rId5"/>
     <sheet name="Parameters" sheetId="6" r:id="rId6"/>
-    <sheet name="Interactions" sheetId="5" r:id="rId7"/>
-    <sheet name="Cascades" sheetId="7" r:id="rId8"/>
-    <sheet name="Plots" sheetId="8" r:id="rId9"/>
+    <sheet name="Cascades" sheetId="10" r:id="rId7"/>
   </sheets>
   <calcPr calcId="179021"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Romesh</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{32DD1623-256E-410E-A864-AB07B61C4590}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Romesh:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Use the code name to assign Compartments, Characteristics, and Parameters to a particular sheet in the databook</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{02FCBC89-37EE-4BD9-AFD7-1CA498C0A432}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Romesh:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This is the name of the sheet that will appear in the 'Sheets' tab of the databook</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
@@ -42,19 +98,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>This column is for the 'code name' of a compartment within a
-population cascade, a state that an entity can exist in that is
-distinct from all other states.
-Examples may include 'sus', 'inf_1', 'rec', etc.
-If entities in the network involve two 'orthogonal' descriptors,
-compartments should combine the status of each state in the title,
-e.g. 'inc_high_edu_hs', to make sure that each entity in a cascade is
-only ever in one state at a time.
-It is possible to bundle independent states as analytical features of
-interest elsewhere in the framework file.
-Note: A code name is a representative key that developers interface
-with (e.g. in scripts and the codebase).
-It should be in lower case without spaces.</t>
+          <t>This is a short 'code name' for the compartment - it should be lower case with no spaces e.g. 'sus'</t>
         </r>
       </text>
     </comment>
@@ -67,24 +111,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>This column is for the 'display name' of a compartment within a
-population cascade, a state that an entity can exist in that is
-distinct from all other states.
-Examples may include 'Susceptible', 'Infected Stage 1', 'Recovered',
-etc.
-If entities in the network involve two 'orthogonal' descriptors,
-compartments should combine the status of each state in the title,
-e.g. 'High Income Earner + Year 12 Education', to make sure that each
-entity in a cascade is only ever in one state at a time.
-It is possible to bundle independent states as analytical features of
-interest elsewhere in the framework file.
-Note: A display name is a representative label that users interface
-with (e.g. in databooks and plots).
-It should be in title or sentence case.</t>
+          <t>The 'Display name' will label the compartment on plots, so it should be descriptive e.g. 'Susceptible'</t>
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{50EA1244-E946-434D-A412-9398789E7050}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{3F46A7DA-FE24-4E1C-9D15-BD3B9B2F2AA3}">
       <text>
         <r>
           <rPr>
@@ -93,24 +124,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>This column is for tagging a compartment as an abstract 'source' state,
-from which entities can flow into the rest of a network.
-Compartment inflows are prohibited, compartment size is meaningless
-and, accordingly, compartment outflows cannot be specified in relative
-format.
-This tag should only be enabled for sources of network flows that are
-not intrinsically bound by size, e.g. births or immigration.
-Flows from sources can still be dependent on other variables in the
-cascade, e.g. if births are controlled by parental population size,
-while migrations between populations are considered transfers,
-i.e. between sets of compartments, and do not involve source nodes.
-Note: This tag is only enabled for a compartment by marking the
-corresponding cell 'y'.
-Anything else, including keeping the cell blank, disables the tag.</t>
+          <t>Select whether you can adjust this compartment in calibration - default is 'n' (cannot calibrate)</t>
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{4B1D614A-6995-4BC4-9139-ADC85A780737}">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{69690E77-E19A-4C62-A1A8-7A79BC1C6D8C}">
       <text>
         <r>
           <rPr>
@@ -119,123 +137,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>This column is for tagging a compartment as an abstract 'sink' state,
-into which entities can flow from the rest of a network.
-Compartment outflows are prohibited and compartment size denotes
-the accumulation of all inflowing entities from the start of
-simulation, the utility of which the user must judge on their own.
-This tag should only be enabled for sinks of network flows that mark
-the exit of entities from further involvement in a cascade, e.g. deaths
-and emigration.
-Migrations between populations are considered transfers, i.e. between
-sets of compartments, and do not involve sink nodes.
-Note: This tag is only enabled for a compartment by marking the
-corresponding cell 'y'.
-Anything else, including keeping the cell blank, disables the tag.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{DB56E746-A899-4F16-8FAE-6600FA84B075}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column is for tagging a compartment as an abstract 'junction'
-state, commonly used to control the aggregation and disaggregation of
-network flows.
-These special nodes are designed to empty out their contents
-immediately after collecting inflow, meaning that they will never
-accumulate any entities at any point in time.
-Accordingly, compartment size is always zero and there must always be
-at least one compartment outflow, each of which must be specified in
-weighted format.
-Inflowing entities will be flushed out to connected states in
-proportion with the weights of the outflowing transitions.
-Models using junctions must be well designed, as a recursion limit will
-break networks involving endless cycles during simulation runtime.
-Note: This tag is only enabled for a compartment by marking the
-corresponding cell 'y'.
-Anything else, including keeping the cell blank, disables the tag.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{B4B78201-E703-45F2-B8E3-C4BE043769F5}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column determines how important user-provided values for this
-compartment are to setting up the initial state of a model.
-In general, the column value should be '1' if model construction
-directly depends on what the user provides for compartment size.
-It should be '0' if supplied values are only for calibration or
-note-keeping purposes.
-In this latter case, the linear-algebra method of setting up
-compartment sizes may complain about an 'under-determined' system
-during a model run.
-To avoid this, every zero-weighted compartment should be matched
-by a 'characteristic' defined in a later spreadsheet that includes
-this compartment and is not weighted zero for setup weight.
-Note: Default value, i.e. a blank cell, is '1'.
-Framework file parsing should also warn the user about a compartment
-with nonzero setup weight that is suppressed in the databook, i.e.
-has a databook order of '-1'.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{3F46A7DA-FE24-4E1C-9D15-BD3B9B2F2AA3}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column marks whether compartment size data can be rescaled
-during model calibration processes.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{69690E77-E19A-4C62-A1A8-7A79BC1C6D8C}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column optionally marks whether a data-input section should
-appear for this compartment in a custom databook sheet, if allowed
-to appear at all according to 'databook order'.
-Each value should be a code name for a desired page defined in
-the 'custom databook pages' worksheet page.
-If a cell is left empty, the enabled data-input section should appear
-in a default databook page dedicated to state variables.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{4DCCC305-48A8-4F07-8F0E-014ED2BF36F9}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column currently denotes whether a databook should request
-values from the user for the historical size of this compartment.
-A value of '-1' suppresses it from appearing in the databook.</t>
+          <t>If you want this compartment to appear in the databook for data entry, then specify one of the datasheet code names (from the 'Databook Pages' sheet) here</t>
         </r>
       </text>
     </comment>
@@ -243,13 +145,13 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Romesh</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{30BE7B3B-8600-4B7D-BACD-39889A358194}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{18A5064E-3D3F-4E47-AB28-08E3744C6678}">
       <text>
         <r>
           <rPr>
@@ -257,7 +159,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Romesh:</t>
         </r>
@@ -266,10 +168,10 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-The transition matrix specifies which parameters govern transitions between compartments. Entries in this matrix should correspond to parameter Code Names (cells will be red if the parameter name cannot be found on the Parameters sheet)</t>
+The transition matrix specifies which transitions exist and which parameter governs them. Transitions go from row to column</t>
         </r>
       </text>
     </comment>
@@ -277,7 +179,7 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
@@ -292,19 +194,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>This column is for the 'code name' of a cascade characteristic,
-which is a set of compartments or, recursively, other characteristics.
-While a characteristic value is typically the population size across
-a set of compartments at a point in time, it can also be normalized by
-another characteristic.
-Defining a characteristic allows the model to track other important
-system state variables beyond the size of just one compartment.
-Examples include 'alive', 'num_inf_all', 'prop_imm', etc.
-Importantly, each compartment defined elsewhere also serves as a
-characteristic.
-Note: A code name is a representative key that developers interface
-with (e.g. in scripts and the codebase).
-It should be in lower case without spaces.</t>
+          <t>This is a short 'code name' for the characteristic - it should be lower case with no spaces e.g. 'all_dx'</t>
         </r>
       </text>
     </comment>
@@ -317,20 +207,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>This column is for the 'display name' of a cascade characteristic,
-which is a set of compartments or, recursively, other characteristics.
-While a characteristic value is typically the population size across
-a set of compartments at a point in time, it can also be normalized by
-another characteristic.
-Defining a characteristic allows the model to track other important
-system state variables beyond the size of just one compartment.
-Examples include 'Number of People Alive', 'Number of Infections Across
-All Strains', 'Proportion of People Immune', etc.
-Importantly, each compartment defined elsewhere also serves as a
-characteristic.
-Note: A display name is a representative label that users interface
-with (e.g. in databooks and plots).
-It should be in title or sentence case.</t>
+          <t xml:space="preserve">The 'Display name' will label the characteristic on plots, so it should be descriptive e.g. 'Aware of diagnosis' </t>
         </r>
       </text>
     </comment>
@@ -343,20 +220,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>This column, and any that immediately follow without a specified
-header, is for the 'components' of a cascade characteristic.
-A component is either a compartment or a characteristic that has
-been previously defined, i.e. in a previous row, and should be
-listed in this (and appropriate subsequent columns) by 'Code Name'.
-For example, characteristic 'infected' may include 'dis_stage_1',
-'dis_stage_2' and 'dis_advanced', where 'dis_advanced' is another
-previously-defined characteristic including 'dis_stage_3' and
-'dis_stage_4'.
-In an example model, 'infected' would track population size summed
-across the four 'dis_stage' states.
-Note: If two or more components are listed in the same column, they
-must be separated by a comma.
-Whitespace is allowable and will be deleted during processing.</t>
+          <t>Specify a comma separated list of compartment and characteristics to include e.g. 'dx,tx'</t>
         </r>
       </text>
     </comment>
@@ -369,11 +233,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>This column defines a 'denominator' attribute for a 'charac' item.</t>
+          <t>If you want this characteristic to correspond to a fraction (e.g. prevalance) then specify the denominator here. For example, a characteristic for prevalance might have components that include all infected people, and a denominator which consists of all people. The denominator should be a single compartment or characteristic, not a list</t>
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{39B7B833-74F0-4AC6-AF4B-699C22909F95}">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{EC0EC08C-D65E-4DFA-A6CF-0EB40DE9D2A2}">
       <text>
         <r>
           <rPr>
@@ -382,11 +246,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>This column defines a 'default_value' attribute for a 'charac' item.</t>
+          <t>Select whether you can adjust this characteristic in calibration - default is 'n' (cannot calibrate)</t>
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{A8C56C78-1F68-424B-8E30-7A6B97DEEFE2}">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{559607C2-31DF-4F19-8B38-ADD8E67B050A}">
       <text>
         <r>
           <rPr>
@@ -395,69 +259,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>This column determines how important user-provided values for this
-characteristic are to setting up the initial state of a model.
-In general, the column value should be '1' if model construction
-directly depends on what the user provides for the characteristic.
-It should be '0' if supplied values are only for calibration or
-note-keeping purposes.
-In this latter case, the linear-algebra method of setting up
-compartment sizes may complain about an 'under-determined' system
-during a model run.
-To avoid this, every compartment that has a nonzero setup weight
-should be included in at least one distinct characteristic.
-Note: Default value, i.e. a blank cell, is '1'.
-Framework file parsing should also warn the user about a characteristic
-with nonzero setup weight that is suppressed in the databook, i.e.
-has a databook order of '-1'.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{EC0EC08C-D65E-4DFA-A6CF-0EB40DE9D2A2}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column marks whether characteristic size data can be rescaled
-during model calibration processes.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{559607C2-31DF-4F19-8B38-ADD8E67B050A}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column optionally marks whether a data-input section should
-appear for this characteristic in a custom databook sheet, if allowed
-to appear at all according to 'databook order'.
-Each value should be a code name for a desired page defined in
-the 'custom databook pages' worksheet page.
-If a cell is left empty, the enabled data-input section should appear
-in a default databook page dedicated to state variables.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{ADDFC9C7-7898-4FFB-896C-C95E74B008F3}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column currently denotes whether a databook should request
-historical values from the user for this characteristic.
-A value of '-1' suppresses it from appearing in the databook.</t>
+          <t>If you want this characteristic to appear in the databook for data entry, then specify one of the datasheet code names (from the 'Databook Pages' sheet) here</t>
         </r>
       </text>
     </comment>
@@ -465,7 +267,7 @@
 </comments>
 </file>
 
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
@@ -480,16 +282,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>This column is for the 'code name' of a cascade parameter.
-The base case is referred to as a transition parameter, referring to
-the flow of entities between compartments.
-However, due to the option of specifying transition rates as functions
-of other parameters, a parameter can be any variable that directly or
-indirectly affects the rate of population change in the network.
-Examples include 'b_rate', 'yes_rate', 'web_cov', etc.
-Note: A code name is a representative key that developers interface
-with (e.g. in scripts and the codebase).
-It should be in lower case without spaces.</t>
+          <t>This is a short 'code name' for the parameter - it should be lower case with no spaces e.g. 'dx_rate'</t>
         </r>
       </text>
     </comment>
@@ -502,17 +295,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>This column is for the 'display name' of a cascade parameter.
-The base case is referred to as a transition parameter, referring to
-the flow of entities between compartments.
-However, due to the option of specifying transition rates as functions
-of other parameters, a parameter can be any variable that directly or
-indirectly affects the rate of population change in the network.
-Examples include 'Birth Rate', 'Treatment Uptake Rate', 'Internet
-Coverage', etc.
-Note: A display name is a representative label that users interface
-with (e.g. in databooks and plots).
-It should be in title or sentence case.</t>
+          <t xml:space="preserve">The 'Display name' will label the parameter on plots, so it should be descriptive e.g. 'Diagnosis rate'' </t>
         </r>
       </text>
     </comment>
@@ -525,7 +308,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>This column defines a 'format' attribute for a 'par' item.</t>
+          <t>Specify the units for the parameter. Generally, it would be 'probability' for the probability of an individual making a transition over a 1 year period, or 'number' for the number of people that transition over a 1 year period</t>
         </r>
       </text>
     </comment>
@@ -538,7 +321,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>This column defines a 'default_value' attribute for a 'par' item.</t>
+          <t>If you specify a default value, it will automatically appear in the databook (but it can be subsequently changed)</t>
         </r>
       </text>
     </comment>
@@ -551,7 +334,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>This column defines a 'min' attribute for a 'par' item.</t>
+          <t>If you specify a minimum value, the parameter will never drop below this value. If included, it would typically be 0</t>
         </r>
       </text>
     </comment>
@@ -564,7 +347,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>This column defines a 'max' attribute for a 'par' item.</t>
+          <t>If you specify a maximum value, the parameter will never exceed this value. A common use would be to ensure that a probability cannot be larger than 1</t>
         </r>
       </text>
     </comment>
@@ -577,7 +360,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>This column defines a 'func' attribute for a 'par' item.</t>
+          <t>If a parameter is computed dynamically as a function, enter the function here</t>
         </r>
       </text>
     </comment>
@@ -590,11 +373,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>This column is for tagging a parameter as a potential program
-impact.
-Note: This tag is only enabled for a parameter by marking the
-corresponding cell 'y'.
-Anything else, including keeping the cell blank, disables the tag.</t>
+          <t>If a parameter is marked as an impact, then it is considered eligible for programs will appear in the program book</t>
         </r>
       </text>
     </comment>
@@ -607,8 +386,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>This column marks whether parameter data can be rescaled
-during model calibration processes.</t>
+          <t>Select whether you can adjust this parameter in calibration - default is 'n' (cannot calibrate)</t>
         </r>
       </text>
     </comment>
@@ -621,28 +399,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>This column optionally marks whether a data-input section should
-appear for this parameter in a custom databook sheet, if allowed
-to appear at all according to 'databook order'.
-Each value should be a code name for a desired page defined in
-the 'custom databook pages' worksheet page.
-If a cell is left empty, the enabled data-input section should appear
-in a default databook page dedicated to parameters.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{F4694702-1A69-4233-A84B-A75E88284228}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column currently denotes whether a databook should request
-historical values from the user for this parameter.
-A value of '-1' suppresses it from appearing in the databook.</t>
+          <t>If you want this parameter to appear in the databook for data entry, then specify one of the datasheet code names (from the 'Databook Pages' sheet) here</t>
         </r>
       </text>
     </comment>
@@ -650,71 +407,57 @@
 </comments>
 </file>
 
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author/>
+    <author>Romesh</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{162B0863-E71C-4603-A693-15E6A2B23038}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{549EE204-B723-4890-A669-72EF2079298D}">
       <text>
         <r>
           <rPr>
-            <sz val="8"/>
+            <b/>
+            <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>This column is for the 'code name' of a population interaction.
-These are special parameters that do not store values per population
-but per pairs of populations, specifically relating to how a source
-population interacts with a target population.
-Examples may include 'w_ctc', 'sex_partners', etc.
-The values that users provide for these matrix parameters, possibly
-time-dependent, can be propagated into population parameters by
-special functions such as 'srcpopavg'.
-Refer to documentation for more details.
-Note: A display name is a representative label that users interface
-with (e.g. in databooks and plots).
-It should be in title or sentence case.</t>
+          <t>Romesh:</t>
         </r>
-      </text>
-    </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{FC00BD5D-BBD8-48DF-8AE7-162658709D7A}">
-      <text>
         <r>
           <rPr>
-            <sz val="8"/>
+            <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>This column is for the 'display name' of a population interaction.
-These are special parameters that do not store values per population
-but per pairs of populations, specifically relating to how a source
-population interacts with a target population.
-Examples may include 'Contact weighting', 'Number of sex partners',
-etc.
-The values that users provide for these matrix parameters, possibly
-time-dependent, can be propagated into population parameters by
-special functions such as 'srcpopavg'.
-Refer to documentation for more details.
-Note: A display name is a representative label that users interface
-with (e.g. in databooks and plots).
-It should be in title or sentence case.</t>
+          <t xml:space="preserve">
+Specify the name of your cascade in this cell. In the cells below, specify the names of your cascade's stages</t>
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{ED07D9E4-694E-4387-BFA2-CAB6F8A058EC}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{B661C074-8D88-4DA5-AC0B-7DB040256031}">
       <text>
         <r>
           <rPr>
-            <sz val="8"/>
+            <b/>
+            <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>This column defines a 'default_value' attribute for a 'interpop' item.</t>
+          <t>Romesh:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+In this column, specify which compartments and characteristics make up each cascade stage. You should specify them as a comma separated list of code names e.g., 'sus, inf, rec'</t>
         </r>
       </text>
     </comment>
@@ -723,13 +466,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="54">
-  <si>
-    <t>Datasheet Code Name</t>
-  </si>
-  <si>
-    <t>Datasheet Title</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
   <si>
     <t>Code Name</t>
   </si>
@@ -737,46 +474,10 @@
     <t>Display Name</t>
   </si>
   <si>
-    <t>Compartment 1</t>
-  </si>
-  <si>
-    <t>Compartment 2</t>
-  </si>
-  <si>
-    <t>Is Source</t>
-  </si>
-  <si>
-    <t>Is Sink</t>
-  </si>
-  <si>
-    <t>Is Junction</t>
-  </si>
-  <si>
-    <t>Default Value</t>
-  </si>
-  <si>
-    <t>Setup Weight</t>
-  </si>
-  <si>
     <t>Can Calibrate</t>
   </si>
   <si>
     <t>Databook Page</t>
-  </si>
-  <si>
-    <t>Databook Order</t>
-  </si>
-  <si>
-    <t>charac_1</t>
-  </si>
-  <si>
-    <t>charac_2</t>
-  </si>
-  <si>
-    <t>Characteristic 1</t>
-  </si>
-  <si>
-    <t>Characteristic 2</t>
   </si>
   <si>
     <t>Components</t>
@@ -788,91 +489,16 @@
     <t>Format</t>
   </si>
   <si>
-    <t>Minimum Value</t>
-  </si>
-  <si>
-    <t>Maximum Value</t>
-  </si>
-  <si>
     <t>Function</t>
-  </si>
-  <si>
-    <t>Is Impact</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Quantities</t>
-  </si>
-  <si>
-    <t>Aggregate pops</t>
-  </si>
-  <si>
-    <t>Plot Group</t>
-  </si>
-  <si>
-    <t>par1</t>
-  </si>
-  <si>
-    <t>par2</t>
-  </si>
-  <si>
-    <t>comp2</t>
-  </si>
-  <si>
-    <t>parameters</t>
-  </si>
-  <si>
-    <t>state_variables</t>
-  </si>
-  <si>
-    <t>State Variables</t>
   </si>
   <si>
     <t>Parameters</t>
   </si>
   <si>
-    <t>comp1</t>
-  </si>
-  <si>
-    <t>main cascade</t>
-  </si>
-  <si>
     <t>Constituents</t>
   </si>
   <si>
-    <t>Stage 1</t>
-  </si>
-  <si>
-    <t>Stage 2</t>
-  </si>
-  <si>
-    <t>series</t>
-  </si>
-  <si>
-    <t>alive</t>
-  </si>
-  <si>
-    <t>both</t>
-  </si>
-  <si>
-    <t>{'All':['comp1','comp2']}</t>
-  </si>
-  <si>
     <t>Transition Matrix</t>
-  </si>
-  <si>
-    <t>Parameter 1</t>
-  </si>
-  <si>
-    <t>Parameter 2</t>
-  </si>
-  <si>
-    <t>interaction_1</t>
-  </si>
-  <si>
-    <t>Interaction 1</t>
   </si>
   <si>
     <t>Name</t>
@@ -885,6 +511,93 @@
   </si>
   <si>
     <t>This is a template cascade</t>
+  </si>
+  <si>
+    <t>stocks</t>
+  </si>
+  <si>
+    <t>flows</t>
+  </si>
+  <si>
+    <t>Stocks</t>
+  </si>
+  <si>
+    <t>Flows</t>
+  </si>
+  <si>
+    <t>Instructions</t>
+  </si>
+  <si>
+    <t>Page Overview</t>
+  </si>
+  <si>
+    <t>Databook Pages</t>
+  </si>
+  <si>
+    <t>Compartments</t>
+  </si>
+  <si>
+    <t>Transitions</t>
+  </si>
+  <si>
+    <t>Characteristics</t>
+  </si>
+  <si>
+    <t>Specify groups of people (e.g. groups of compartments) for data entry</t>
+  </si>
+  <si>
+    <t>Cascade name</t>
+  </si>
+  <si>
+    <t>Cascades</t>
+  </si>
+  <si>
+    <t>Use the Cascades sheet to define the cascade if it is more complex than just all characteristics in sequence</t>
+  </si>
+  <si>
+    <t>Define how to compute the flows between compartments</t>
+  </si>
+  <si>
+    <t>Specify which transitions between compartments are possible</t>
+  </si>
+  <si>
+    <t>Specify the states that an individual can be in - an individual is only ever in one compartment at a time</t>
+  </si>
+  <si>
+    <t>Specify which worksheets will be present in the databook</t>
+  </si>
+  <si>
+    <t>Code name</t>
+  </si>
+  <si>
+    <t>Datasheet code name</t>
+  </si>
+  <si>
+    <t>Datasheet title</t>
+  </si>
+  <si>
+    <t>Display name</t>
+  </si>
+  <si>
+    <t>Use this file to specify the structure of your model. Any extra sheets will be ignored, so you can include other information in them</t>
+  </si>
+  <si>
+    <t>Default value</t>
+  </si>
+  <si>
+    <t>Minimum value</t>
+  </si>
+  <si>
+    <t>Maximum value</t>
+  </si>
+  <si>
+    <t>Is impact</t>
+  </si>
+  <si>
+    <t>Can calibrate</t>
+  </si>
+  <si>
+    <t>Databook page</t>
   </si>
 </sst>
 </file>
@@ -917,14 +630,14 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -947,7 +660,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -959,9 +672,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -969,7 +679,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="11">
     <dxf>
       <fill>
         <patternFill>
@@ -1015,6 +725,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -1023,20 +740,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1391,32 +1094,95 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.5703125" customWidth="1"/>
-    <col min="2" max="2" width="74.85546875" customWidth="1"/>
+    <col min="2" max="2" width="97.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="234.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>53</v>
+      <c r="A2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1426,14 +1192,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1444,35 +1210,36 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="11" priority="1">
+    <cfRule type="expression" dxfId="10" priority="1">
       <formula>AND(A1&lt;&gt;"",NOT(B1&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1481,94 +1248,59 @@
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" style="4" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="2" customWidth="1"/>
+    <col min="3" max="5" width="18.7109375" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
       <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C3" s="2"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="10" priority="4">
+    <cfRule type="expression" dxfId="9" priority="4">
       <formula>AND(A1&lt;&gt;"",NOT(B1&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H1048576">
-    <cfRule type="expression" dxfId="9" priority="2">
-      <formula>AND(I2&lt;&gt;"",NOT(H2&lt;&gt;""))</formula>
+  <conditionalFormatting sqref="D2:D1048576">
+    <cfRule type="expression" dxfId="7" priority="7">
+      <formula>AND(#REF!&lt;&gt;"",NOT(D2&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:E1048576 G1:G1048576" xr:uid="{EFA3D3D9-56A8-43F0-A737-1EDBC3038312}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{EFA3D3D9-56A8-43F0-A737-1EDBC3038312}">
       <formula1>"n,y"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1580,7 +1312,7 @@
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="1" id="{0238372B-F012-4B98-A58B-305EDC0BD903}">
-            <xm:f>AND(H2&lt;&gt;"",ISERROR(MATCH(H2,'Databook Pages'!$A:$A,0)))</xm:f>
+            <xm:f>AND(D2&lt;&gt;"",ISERROR(MATCH(D2,'Databook Pages'!$A:$A,0)))</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -1589,7 +1321,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>H2:H1048576</xm:sqref>
+          <xm:sqref>D2:D1048576</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1599,7 +1331,7 @@
           <x14:formula1>
             <xm:f>'Databook Pages'!$A$2:$A$9999</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H1048576</xm:sqref>
+          <xm:sqref>D2:D1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1615,7 +1347,7 @@
   <dimension ref="A1:OH398"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1625,15 +1357,15 @@
   <sheetData>
     <row r="1" spans="1:398" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="B1" s="3" t="str">
         <f>IF(Compartments!$A2&lt;&gt;"",Compartments!$A2,"")</f>
-        <v>comp1</v>
+        <v/>
       </c>
       <c r="C1" s="3" t="str">
         <f>IF(Compartments!$A3&lt;&gt;"",Compartments!$A3,"")</f>
-        <v>comp2</v>
+        <v/>
       </c>
       <c r="D1" s="3" t="str">
         <f>IF(Compartments!$A4&lt;&gt;"",Compartments!$A4,"")</f>
@@ -3219,13 +2951,13 @@
     <row r="2" spans="1:398" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="str">
         <f>IF(Compartments!$A2&lt;&gt;"",Compartments!$A2,"")</f>
-        <v>comp1</v>
+        <v/>
       </c>
     </row>
     <row r="3" spans="1:398" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="str">
         <f>IF(Compartments!$A3&lt;&gt;"",Compartments!$A3,"")</f>
-        <v>comp2</v>
+        <v/>
       </c>
     </row>
     <row r="4" spans="1:398" x14ac:dyDescent="0.25">
@@ -5628,10 +5360,10 @@
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5640,79 +5372,50 @@
     <col min="2" max="2" width="16.85546875" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="2" customWidth="1"/>
+    <col min="6" max="7" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
       <c r="F2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
+      <c r="G2" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="expression" dxfId="6" priority="6">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>AND(A2&lt;&gt;"",NOT(B2&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H1048576">
-    <cfRule type="expression" dxfId="5" priority="5">
-      <formula>AND(I2&lt;&gt;"",NOT(H2&lt;&gt;""))</formula>
+  <conditionalFormatting sqref="F2:F1048576">
+    <cfRule type="expression" dxfId="3" priority="8">
+      <formula>AND(#REF!&lt;&gt;"",NOT(F2&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576" xr:uid="{3FB7A4A5-B63C-489E-8DB0-DCA9DC6C3431}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576" xr:uid="{3FB7A4A5-B63C-489E-8DB0-DCA9DC6C3431}">
       <formula1>"n,y"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5724,7 +5427,7 @@
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="1" id="{B070FBDA-10C1-45BC-AA32-DA4BD51EB2DD}">
-            <xm:f>AND(H2&lt;&gt;"",ISERROR(MATCH(H2,'Databook Pages'!$A:$A,0)))</xm:f>
+            <xm:f>AND(F2&lt;&gt;"",ISERROR(MATCH(F2,'Databook Pages'!$A:$A,0)))</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -5733,7 +5436,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>H2:H1048576</xm:sqref>
+          <xm:sqref>F2:F1048576</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -5743,7 +5446,7 @@
           <x14:formula1>
             <xm:f>'Databook Pages'!$A$2:$A$9999</xm:f>
           </x14:formula1>
-          <xm:sqref>H1:H1048576</xm:sqref>
+          <xm:sqref>F1:F1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5756,10 +5459,10 @@
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5772,83 +5475,67 @@
     <col min="8" max="8" width="10.7109375" style="2" customWidth="1"/>
     <col min="9" max="9" width="14.7109375" style="2" customWidth="1"/>
     <col min="10" max="10" width="14.7109375" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" t="s">
-        <v>46</v>
-      </c>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" t="s">
-        <v>47</v>
-      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>AND(A1&lt;&gt;"",NOT(B1&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J1048576">
-    <cfRule type="expression" dxfId="2" priority="2">
-      <formula>AND(K2&lt;&gt;"",NOT(J2&lt;&gt;""))</formula>
+    <cfRule type="expression" dxfId="0" priority="9">
+      <formula>AND(#REF!&lt;&gt;"",NOT(J2&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:I1048576" xr:uid="{7CB7BECB-8CCA-402C-8209-B57AEC65D6EC}">
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:I1048576" xr:uid="{7CB7BECB-8CCA-402C-8209-B57AEC65D6EC}">
       <formula1>"n,y"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Code names must be unique" error="Parameter code names must be unique" sqref="A1:A1048576" xr:uid="{E6E68E87-C2E4-4D80-BD6F-D69CE5F2A8E2}">
-      <formula1>COUNTIF(A:A,A1)&lt;2</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Code names must be unique" error="Parameter code names must be unique" sqref="A2:A1048576" xr:uid="{E6E68E87-C2E4-4D80-BD6F-D69CE5F2A8E2}">
+      <formula1>COUNTIF(A:A,A2)&lt;2</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{8BE00A64-F133-4296-8701-DE6AB3B8505B}">
+      <formula1>"probability, number, duration, proportion"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5877,7 +5564,7 @@
           <x14:formula1>
             <xm:f>'Databook Pages'!$A$2:$A$9999</xm:f>
           </x14:formula1>
-          <xm:sqref>J1:J1048576</xm:sqref>
+          <xm:sqref>J2:J1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5886,180 +5573,34 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <sheetPr>
-    <tabColor theme="5" tint="0.79998168889431442"/>
-  </sheetPr>
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45475D22-3C2C-420F-8B01-74A730C6AAB5}">
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>AND(A1&lt;&gt;"",NOT(B1&lt;&gt;""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A1EAFB5-C4B0-491C-B03B-D10386E1B6D4}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="55.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>36</v>
-      </c>
+      <c r="B2" s="4"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>31</v>
-      </c>
+      <c r="B3" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6A2575B-90FD-4432-ABB5-1D1C9A3EC31C}">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="14" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{B6FB0777-9CB4-4E7A-978E-F88EC2A52ADA}">
-      <formula1>"n,y"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>